<commit_message>
[feat] Stage -> Dungeon으로 바꾸고 Stage를 하위 개념으로 바꿈
</commit_message>
<xml_diff>
--- a/DataParser/Monster.xlsx
+++ b/DataParser/Monster.xlsx
@@ -238,11 +238,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Stage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DataId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dungeon</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -576,7 +576,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:J6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -587,7 +587,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -596,7 +596,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>

</xml_diff>